<commit_message>
working code with proper reports and sequential execution
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/EmployeeData.xlsx
+++ b/src/test/resources/Data/EmployeeData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarit\eclipse-workspace\employee-api-tests\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67023F88-16CC-4E2E-9751-2514D2008090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0E5EFB-8F22-4F73-94FE-0D1F360EDBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F0B7B5AE-6266-4CA6-9D41-6C5D1CADB66D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -50,60 +50,12 @@
     <t>qa</t>
   </si>
   <si>
-    <t>ValidateCustomerApiWithValidData</t>
-  </si>
-  <si>
-    <t>ValidateCustomerApiWithInValidData</t>
-  </si>
-  <si>
     <t>dev</t>
   </si>
   <si>
     <t>kia  MALHOTRA J</t>
   </si>
   <si>
-    <t>testGetUserDataSuccess</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>avatar</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>janet.weaver@reqres.in</t>
-  </si>
-  <si>
-    <t>Janet</t>
-  </si>
-  <si>
-    <t>Weaver</t>
-  </si>
-  <si>
-    <t>https://reqres.in/img/faces/2-image.jpg</t>
-  </si>
-  <si>
-    <t>https://reqres.in/#support-heading</t>
-  </si>
-  <si>
-    <t>To keep ReqRes free, contributions towards server costs are appreciated!</t>
-  </si>
-  <si>
     <t>"$%%^</t>
   </si>
   <si>
@@ -116,40 +68,32 @@
     <t>Hiya</t>
   </si>
   <si>
-    <t>ValidateMultipleEmployeecReationSimultatiouslyAndVerifyUniqueIdForEachEmployee</t>
-  </si>
-  <si>
     <t>Dhoni</t>
   </si>
   <si>
     <t>PM</t>
+  </si>
+  <si>
+    <t>TC001_ValidateCustomerApiWithValidData</t>
+  </si>
+  <si>
+    <t>TC002_ValidateCustomerApiWithInValidData</t>
+  </si>
+  <si>
+    <t>TC003_ValidateMultipleEmployeeCReationWithSameDataAndVerifyUniqueIdForEachEmployee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -165,24 +109,10 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FF312540"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF312540"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -208,39 +138,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,176 +487,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A45579F-8418-422F-8A3E-20D8E5EF5099}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.109375" style="4" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="56.109375" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="6" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>2</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>28</v>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F14" r:id="rId1" location="support-heading" display="https://reqres.in/ - support-heading" xr:uid="{8362B298-2848-42B2-A886-1953EE2D9DF7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added data latecy code
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/EmployeeData.xlsx
+++ b/src/test/resources/Data/EmployeeData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarit\eclipse-workspace\employee-api-tests\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0E5EFB-8F22-4F73-94FE-0D1F360EDBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F150A0F-0DF9-4C36-931C-9EB57E93FAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F0B7B5AE-6266-4CA6-9D41-6C5D1CADB66D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>TC003_ValidateMultipleEmployeeCReationWithSameDataAndVerifyUniqueIdForEachEmployee</t>
+  </si>
+  <si>
+    <t>TC004__ValidateCreateAPILatency</t>
+  </si>
+  <si>
+    <t>Popy</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A45579F-8418-422F-8A3E-20D8E5EF5099}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -601,6 +607,27 @@
         <v>11</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>